<commit_message>
Adicionando versoes aos sprint backlog e adicionando pasta de controle para sprint
</commit_message>
<xml_diff>
--- a/Sprint_Backlog/v2.0/Sprint_backlog.xlsx
+++ b/Sprint_Backlog/v2.0/Sprint_backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaique\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaique\Documents\UNIP\ASOO\Fazenda_Urbana\Sprint_Backlog\v2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>Sprint</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>Concluido</t>
+  </si>
+  <si>
+    <t>Em progesso</t>
+  </si>
+  <si>
+    <t>Não iniciado</t>
+  </si>
+  <si>
+    <t>Baixa</t>
   </si>
 </sst>
 </file>
@@ -123,7 +132,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +157,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -169,14 +184,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -462,7 +479,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,14 +493,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -515,7 +532,7 @@
       <c r="C3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="1">
@@ -543,7 +560,7 @@
       <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E5" s="1">
@@ -563,7 +580,7 @@
       <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="1">
@@ -591,13 +608,15 @@
       <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -609,13 +628,15 @@
       <c r="C9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -635,11 +656,15 @@
       <c r="C11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E11" s="1">
         <v>3</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -651,11 +676,15 @@
       <c r="C12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="E12" s="1">
         <v>4</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
@@ -679,7 +708,9 @@
       <c r="E14" s="1">
         <v>4</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -695,7 +726,9 @@
       <c r="E15" s="1">
         <v>3</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -711,7 +744,9 @@
       <c r="E16" s="1">
         <v>5</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -735,7 +770,9 @@
       <c r="E18" s="1">
         <v>5</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -759,7 +796,9 @@
       <c r="E20" s="1">
         <v>1</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>

</xml_diff>